<commit_message>
use RMSE of multiple data points as loss
</commit_message>
<xml_diff>
--- a/ammonia_data.xlsx
+++ b/ammonia_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\GitHub\Parameter-Estimation-BO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2509223-C7C8-48C1-BD13-0D8A8099C53B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978FBEBB-78D1-48CD-83D0-E33E528D100B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11430" yWindow="1950" windowWidth="12150" windowHeight="15300" xr2:uid="{1464C18D-A90A-4D35-B2D1-5CAE70CCBB25}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1464C18D-A90A-4D35-B2D1-5CAE70CCBB25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="32">
   <si>
     <t>Run</t>
   </si>
@@ -87,13 +88,58 @@
     <t>*This was modeled as a PFR (200 CSTR's)</t>
   </si>
   <si>
+    <t> Temp.</t>
+  </si>
+  <si>
+    <t>[K]</t>
+  </si>
+  <si>
+    <t> Conversion</t>
+  </si>
+  <si>
+    <t> Rate</t>
+  </si>
+  <si>
+    <t>[TOF]</t>
+  </si>
+  <si>
+    <t>Molar</t>
+  </si>
+  <si>
+    <t>Feed</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>[H2:N2]</t>
+  </si>
+  <si>
+    <t> 10.09</t>
+  </si>
+  <si>
+    <t> 13.32</t>
+  </si>
+  <si>
+    <t>Feed ratio (H2:N2)</t>
+  </si>
+  <si>
     <t>Weight</t>
+  </si>
+  <si>
+    <t>Residence time (s)</t>
+  </si>
+  <si>
+    <t>Pressure (atm)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -105,8 +151,9 @@
     <font>
       <sz val="12"/>
       <color rgb="FF222222"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,14 +176,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,201 +501,264 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A0FC752-7FF1-430C-9E59-EC5D7CBD0C57}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="2" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
+        <v>50</v>
+      </c>
+      <c r="D2" s="5">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4">
+        <v>100</v>
+      </c>
+      <c r="F2" s="6">
         <v>1.26</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="3">
+      <c r="G2" s="4">
+        <v>1</v>
+      </c>
+      <c r="H2" s="7">
         <v>-1.17E-2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="J2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L2" t="s">
         <v>1</v>
       </c>
-      <c r="M2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="N2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
+        <v>50</v>
+      </c>
+      <c r="D3" s="5">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4">
+        <v>100</v>
+      </c>
+      <c r="F3" s="6">
         <v>2.86</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="3">
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
+      <c r="H3" s="7">
         <v>-2.5100000000000001E-2</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="I3" s="4"/>
+      <c r="J3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L3" t="s">
         <v>1</v>
       </c>
-      <c r="M3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="N3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
+        <v>50</v>
+      </c>
+      <c r="D4" s="5">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4">
+        <v>100</v>
+      </c>
+      <c r="F4" s="6">
         <v>6.97</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="3">
+      <c r="G4" s="4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7">
         <v>-5.7000000000000002E-2</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="I4" s="4"/>
+      <c r="J4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L4" t="s">
         <v>1</v>
       </c>
-      <c r="M4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="N4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3">
+        <v>50</v>
+      </c>
+      <c r="D5" s="5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="4">
+        <v>100</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3">
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7">
         <v>-9.2499999999999999E-2</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="I5" s="4"/>
+      <c r="J5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3">
+        <v>50</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4">
+        <v>100</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6">
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4">
         <v>-0.13300000000000001</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
-        <v>1</v>
-      </c>
-      <c r="K6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="I6" s="4"/>
+      <c r="J6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" t="s">
         <v>1</v>
       </c>
       <c r="N6" t="s">
@@ -654,43 +767,470 @@
       <c r="O6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="Q6" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3">
+        <v>50</v>
+      </c>
+      <c r="D7" s="5">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4">
+        <v>100</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7">
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4">
         <v>-0.153</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
-        <v>1</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="I7" s="4"/>
+      <c r="J7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" t="s">
         <v>1</v>
       </c>
       <c r="N7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>50</v>
+      </c>
+      <c r="D8" s="5">
+        <v>2</v>
+      </c>
+      <c r="E8" s="4">
+        <v>100</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
+        <v>-0.105</v>
+      </c>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3">
+        <v>50</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4">
+        <v>100</v>
+      </c>
+      <c r="F9" s="6">
+        <v>7.51</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
+        <v>-0.11700000000000001</v>
+      </c>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3">
+        <v>50</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="4">
+        <v>100</v>
+      </c>
+      <c r="F10" s="6">
+        <v>5.29</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4">
+        <v>-0.11</v>
+      </c>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3">
+        <v>50</v>
+      </c>
+      <c r="D11" s="5">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E11" s="4">
+        <v>100</v>
+      </c>
+      <c r="F11" s="6">
+        <v>4.05</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="7">
+        <v>-9.4500000000000001E-2</v>
+      </c>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3">
+        <v>50</v>
+      </c>
+      <c r="D12" s="5">
+        <f>4</f>
+        <v>4</v>
+      </c>
+      <c r="E12" s="4">
+        <v>100</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="H12" s="7">
+        <v>-8.2900000000000001E-2</v>
+      </c>
+      <c r="I12" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB44FCEE-839F-49C1-A50B-1EEC7602655F}">
+  <dimension ref="A1:T7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" t="s">
+        <v>1</v>
+      </c>
+      <c r="S5" t="s">
+        <v>1</v>
+      </c>
+      <c r="T5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add in temperature dependence
</commit_message>
<xml_diff>
--- a/ammonia_data.xlsx
+++ b/ammonia_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\GitHub\Parameter-Estimation-BO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerhard\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978FBEBB-78D1-48CD-83D0-E33E528D100B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B1FA07-AD5A-497A-9155-D62DFB7C531B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1464C18D-A90A-4D35-B2D1-5CAE70CCBB25}"/>
+    <workbookView xWindow="30" yWindow="0" windowWidth="28710" windowHeight="15555" xr2:uid="{1464C18D-A90A-4D35-B2D1-5CAE70CCBB25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="21">
   <si>
     <t>Run</t>
   </si>
@@ -43,33 +43,6 @@
     <t> </t>
   </si>
   <si>
-    <t> 523.00</t>
-  </si>
-  <si>
-    <t> 553.00</t>
-  </si>
-  <si>
-    <t> 593.00</t>
-  </si>
-  <si>
-    <t> 623.00</t>
-  </si>
-  <si>
-    <t> 11.89</t>
-  </si>
-  <si>
-    <t> 653.00</t>
-  </si>
-  <si>
-    <t> 17.94</t>
-  </si>
-  <si>
-    <t> 673.00</t>
-  </si>
-  <si>
-    <t> 21.20</t>
-  </si>
-  <si>
     <t>  </t>
   </si>
   <si>
@@ -82,9 +55,6 @@
     <t> Rate (TOF)</t>
   </si>
   <si>
-    <t>*P = 50 atm, V = 1 cm3, q = 0.01 cm3/sec (@ rxn conditions), Molar feed ratio = 3:1 (H2:N2)</t>
-  </si>
-  <si>
     <t>*This was modeled as a PFR (200 CSTR's)</t>
   </si>
   <si>
@@ -115,12 +85,6 @@
     <t>[H2:N2]</t>
   </si>
   <si>
-    <t> 10.09</t>
-  </si>
-  <si>
-    <t> 13.32</t>
-  </si>
-  <si>
     <t>Feed ratio (H2:N2)</t>
   </si>
   <si>
@@ -131,6 +95,9 @@
   </si>
   <si>
     <t>Pressure (atm)</t>
+  </si>
+  <si>
+    <t>*V = 1 cm3, q = 0.01 cm3/sec (@ rxn conditions)</t>
   </si>
 </sst>
 </file>
@@ -176,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -187,6 +154,18 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,17 +480,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A0FC752-7FF1-430C-9E59-EC5D7CBD0C57}">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -520,86 +500,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>503</v>
+      </c>
+      <c r="C2" s="3">
+        <v>50</v>
+      </c>
+      <c r="D2" s="5">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4">
+        <v>100</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="G2" s="11">
+        <v>1</v>
+      </c>
+      <c r="H2" s="12">
+        <v>-6.4400000000000004E-3</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="C2" s="3">
-        <v>50</v>
-      </c>
-      <c r="D2" s="5">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4">
-        <v>100</v>
-      </c>
-      <c r="F2" s="6">
-        <v>1.26</v>
-      </c>
-      <c r="G2" s="4">
-        <v>1</v>
-      </c>
-      <c r="H2" s="7">
-        <v>-1.17E-2</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
+      <c r="B3" s="3">
+        <v>513</v>
       </c>
       <c r="C3" s="3">
         <v>50</v>
@@ -610,41 +571,24 @@
       <c r="E3" s="4">
         <v>100</v>
       </c>
-      <c r="F3" s="6">
-        <v>2.86</v>
-      </c>
-      <c r="G3" s="4">
-        <v>1</v>
-      </c>
-      <c r="H3" s="7">
-        <v>-2.5100000000000001E-2</v>
+      <c r="F3" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="G3" s="11">
+        <v>1</v>
+      </c>
+      <c r="H3" s="12">
+        <v>-8.7600000000000004E-3</v>
       </c>
       <c r="I3" s="4"/>
-      <c r="J3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" t="s">
-        <v>1</v>
-      </c>
-      <c r="O3" t="s">
-        <v>1</v>
-      </c>
-      <c r="P3" t="s">
-        <v>1</v>
-      </c>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
+      <c r="B4" s="8">
+        <v>523</v>
       </c>
       <c r="C4" s="3">
         <v>50</v>
@@ -656,21 +600,18 @@
         <v>100</v>
       </c>
       <c r="F4" s="6">
-        <v>6.97</v>
-      </c>
-      <c r="G4" s="4">
+        <v>1.26</v>
+      </c>
+      <c r="G4" s="11">
         <v>1</v>
       </c>
       <c r="H4" s="7">
-        <v>-5.7000000000000002E-2</v>
-      </c>
-      <c r="I4" s="4"/>
+        <v>-1.17E-2</v>
+      </c>
       <c r="J4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="K4" s="1"/>
       <c r="L4" t="s">
         <v>1</v>
       </c>
@@ -688,98 +629,66 @@
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="9">
+        <v>533</v>
+      </c>
+      <c r="C5" s="3">
+        <v>50</v>
+      </c>
+      <c r="D5" s="5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="4">
+        <v>100</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1.68</v>
+      </c>
+      <c r="G5" s="11">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7">
+        <v>-1.5299999999999999E-2</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="C5" s="3">
-        <v>50</v>
-      </c>
-      <c r="D5" s="5">
-        <v>3</v>
-      </c>
-      <c r="E5" s="4">
-        <v>100</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="B6" s="9">
+        <v>543</v>
+      </c>
+      <c r="C6" s="3">
+        <v>50</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4">
+        <v>100</v>
+      </c>
+      <c r="F6" s="6">
+        <v>2.21</v>
+      </c>
+      <c r="G6" s="11">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7">
+        <v>-1.9800000000000002E-2</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="G5" s="4">
-        <v>1</v>
-      </c>
-      <c r="H5" s="7">
-        <v>-9.2499999999999999E-2</v>
-      </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M5" t="s">
-        <v>1</v>
-      </c>
-      <c r="N5" t="s">
-        <v>1</v>
-      </c>
-      <c r="O5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3">
-        <v>50</v>
-      </c>
-      <c r="D6" s="5">
-        <v>3</v>
-      </c>
-      <c r="E6" s="4">
-        <v>100</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="4">
-        <v>1</v>
-      </c>
-      <c r="H6" s="4">
-        <v>-0.13300000000000001</v>
-      </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M6" t="s">
-        <v>1</v>
-      </c>
-      <c r="N6" t="s">
-        <v>1</v>
-      </c>
-      <c r="O6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>1</v>
-      </c>
-      <c r="R6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>9</v>
+      <c r="B7" s="8">
+        <v>553</v>
       </c>
       <c r="C7" s="3">
         <v>50</v>
@@ -790,23 +699,21 @@
       <c r="E7" s="4">
         <v>100</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="4">
-        <v>1</v>
-      </c>
-      <c r="H7" s="4">
-        <v>-0.153</v>
+      <c r="F7" s="6">
+        <v>2.86</v>
+      </c>
+      <c r="G7" s="11">
+        <v>1</v>
+      </c>
+      <c r="H7" s="7">
+        <v>-2.5100000000000001E-2</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="K7" s="1"/>
+      <c r="L7" t="s">
         <v>1</v>
       </c>
       <c r="N7" t="s">
@@ -815,146 +722,589 @@
       <c r="O7" t="s">
         <v>1</v>
       </c>
-      <c r="Q7" t="s">
-        <v>11</v>
+      <c r="P7" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>5</v>
+      <c r="B8" s="9">
+        <v>563</v>
       </c>
       <c r="C8" s="3">
         <v>50</v>
       </c>
       <c r="D8" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" s="4">
         <v>100</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="4">
-        <v>1</v>
-      </c>
-      <c r="H8" s="4">
-        <v>-0.105</v>
+      <c r="F8" s="6">
+        <v>3.65</v>
+      </c>
+      <c r="G8" s="11">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7">
+        <v>-3.1399999999999997E-2</v>
       </c>
       <c r="I8" s="4"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>5</v>
+      <c r="B9" s="9">
+        <v>573</v>
       </c>
       <c r="C9" s="3">
         <v>50</v>
       </c>
       <c r="D9" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E9" s="4">
         <v>100</v>
       </c>
       <c r="F9" s="6">
-        <v>7.51</v>
-      </c>
-      <c r="G9" s="4">
-        <v>1</v>
-      </c>
-      <c r="H9" s="4">
-        <v>-0.11700000000000001</v>
+        <v>4.59</v>
+      </c>
+      <c r="G9" s="11">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7">
+        <v>-3.8800000000000001E-2</v>
       </c>
       <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>5</v>
+      <c r="B10" s="9">
+        <v>583</v>
       </c>
       <c r="C10" s="3">
         <v>50</v>
       </c>
       <c r="D10" s="5">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="E10" s="4">
         <v>100</v>
       </c>
       <c r="F10" s="6">
-        <v>5.29</v>
-      </c>
-      <c r="G10" s="4">
-        <v>1</v>
-      </c>
-      <c r="H10" s="4">
-        <v>-0.11</v>
+        <v>5.69</v>
+      </c>
+      <c r="G10" s="11">
+        <v>1</v>
+      </c>
+      <c r="H10" s="7">
+        <v>-4.7300000000000002E-2</v>
       </c>
       <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>5</v>
+      <c r="B11" s="8">
+        <v>593</v>
       </c>
       <c r="C11" s="3">
         <v>50</v>
       </c>
       <c r="D11" s="5">
-        <f>1/3</f>
-        <v>0.33333333333333331</v>
+        <v>3</v>
       </c>
       <c r="E11" s="4">
         <v>100</v>
       </c>
       <c r="F11" s="6">
-        <v>4.05</v>
-      </c>
-      <c r="G11" s="4">
+        <v>6.97</v>
+      </c>
+      <c r="G11" s="11">
         <v>1</v>
       </c>
       <c r="H11" s="7">
-        <v>-9.4500000000000001E-2</v>
+        <v>-5.7000000000000002E-2</v>
       </c>
       <c r="I11" s="4"/>
+      <c r="J11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1</v>
+      </c>
+      <c r="O11" t="s">
+        <v>1</v>
+      </c>
+      <c r="P11" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>5</v>
+      <c r="B12" s="9">
+        <v>603</v>
       </c>
       <c r="C12" s="3">
         <v>50</v>
       </c>
       <c r="D12" s="5">
+        <v>3</v>
+      </c>
+      <c r="E12" s="4">
+        <v>100</v>
+      </c>
+      <c r="F12">
+        <v>8.43</v>
+      </c>
+      <c r="G12" s="11">
+        <v>1</v>
+      </c>
+      <c r="H12" s="13">
+        <v>-6.7799999999999999E-2</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="M12" t="s">
+        <v>1</v>
+      </c>
+      <c r="N12" t="s">
+        <v>1</v>
+      </c>
+      <c r="O12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="9">
+        <v>613</v>
+      </c>
+      <c r="C13" s="3">
+        <v>50</v>
+      </c>
+      <c r="D13" s="5">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4">
+        <v>100</v>
+      </c>
+      <c r="F13">
+        <v>10.07</v>
+      </c>
+      <c r="G13" s="11">
+        <v>1</v>
+      </c>
+      <c r="H13" s="13">
+        <v>-7.9600000000000004E-2</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1"/>
+      <c r="M13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N13" t="s">
+        <v>1</v>
+      </c>
+      <c r="O13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>1</v>
+      </c>
+      <c r="R13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8">
+        <v>623</v>
+      </c>
+      <c r="C14" s="3">
+        <v>50</v>
+      </c>
+      <c r="D14" s="5">
+        <v>3</v>
+      </c>
+      <c r="E14" s="4">
+        <v>100</v>
+      </c>
+      <c r="F14" s="6">
+        <v>11.89</v>
+      </c>
+      <c r="G14" s="11">
+        <v>1</v>
+      </c>
+      <c r="H14" s="7">
+        <v>-9.2499999999999999E-2</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="J14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1"/>
+      <c r="M14" t="s">
+        <v>1</v>
+      </c>
+      <c r="N14" t="s">
+        <v>1</v>
+      </c>
+      <c r="O14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="9">
+        <v>633</v>
+      </c>
+      <c r="C15" s="3">
+        <v>50</v>
+      </c>
+      <c r="D15" s="5">
+        <v>3</v>
+      </c>
+      <c r="E15" s="4">
+        <v>100</v>
+      </c>
+      <c r="F15">
+        <v>13.85</v>
+      </c>
+      <c r="G15" s="11">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>-0.106</v>
+      </c>
+      <c r="I15" s="4"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="9">
+        <v>643</v>
+      </c>
+      <c r="C16" s="3">
+        <v>50</v>
+      </c>
+      <c r="D16" s="5">
+        <v>3</v>
+      </c>
+      <c r="E16" s="4">
+        <v>100</v>
+      </c>
+      <c r="F16">
+        <v>15.9</v>
+      </c>
+      <c r="G16" s="11">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>-0.12</v>
+      </c>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8">
+        <v>653</v>
+      </c>
+      <c r="C17" s="3">
+        <v>50</v>
+      </c>
+      <c r="D17" s="5">
+        <v>3</v>
+      </c>
+      <c r="E17" s="4">
+        <v>100</v>
+      </c>
+      <c r="F17" s="6">
+        <v>17.940000000000001</v>
+      </c>
+      <c r="G17" s="11">
+        <v>1</v>
+      </c>
+      <c r="H17" s="4">
+        <v>-0.13300000000000001</v>
+      </c>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="9">
+        <v>663</v>
+      </c>
+      <c r="C18" s="3">
+        <v>50</v>
+      </c>
+      <c r="D18" s="5">
+        <v>3</v>
+      </c>
+      <c r="E18" s="4">
+        <v>100</v>
+      </c>
+      <c r="F18">
+        <v>19.8</v>
+      </c>
+      <c r="G18" s="11">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>-0.14499999999999999</v>
+      </c>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="8">
+        <v>673</v>
+      </c>
+      <c r="C19" s="3">
+        <v>50</v>
+      </c>
+      <c r="D19" s="5">
+        <v>3</v>
+      </c>
+      <c r="E19" s="4">
+        <v>100</v>
+      </c>
+      <c r="F19" s="6">
+        <v>21.2</v>
+      </c>
+      <c r="G19" s="11">
+        <v>1</v>
+      </c>
+      <c r="H19" s="4">
+        <v>-0.153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="10">
+        <v>683</v>
+      </c>
+      <c r="C20" s="3">
+        <v>50</v>
+      </c>
+      <c r="D20" s="5">
+        <v>3</v>
+      </c>
+      <c r="E20" s="4">
+        <v>100</v>
+      </c>
+      <c r="F20">
+        <v>21.86</v>
+      </c>
+      <c r="G20" s="11">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>-0.155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="10">
+        <v>693</v>
+      </c>
+      <c r="C21" s="3">
+        <v>50</v>
+      </c>
+      <c r="D21" s="5">
+        <v>3</v>
+      </c>
+      <c r="E21" s="4">
+        <v>100</v>
+      </c>
+      <c r="F21">
+        <v>21.55</v>
+      </c>
+      <c r="G21" s="11">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>-0.151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4">
+        <v>623</v>
+      </c>
+      <c r="C22" s="3">
+        <v>50</v>
+      </c>
+      <c r="D22" s="5">
+        <v>2</v>
+      </c>
+      <c r="E22" s="4">
+        <v>100</v>
+      </c>
+      <c r="F22" s="6">
+        <v>10.09</v>
+      </c>
+      <c r="G22" s="11">
+        <v>1</v>
+      </c>
+      <c r="H22" s="4">
+        <v>-0.105</v>
+      </c>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4">
+        <v>623</v>
+      </c>
+      <c r="C23" s="3">
+        <v>50</v>
+      </c>
+      <c r="D23" s="5">
+        <v>1</v>
+      </c>
+      <c r="E23" s="4">
+        <v>100</v>
+      </c>
+      <c r="F23" s="6">
+        <v>7.51</v>
+      </c>
+      <c r="G23" s="11">
+        <v>1</v>
+      </c>
+      <c r="H23" s="4">
+        <v>-0.11700000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4">
+        <v>623</v>
+      </c>
+      <c r="C24" s="3">
+        <v>50</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E24" s="4">
+        <v>100</v>
+      </c>
+      <c r="F24" s="6">
+        <v>5.29</v>
+      </c>
+      <c r="G24" s="11">
+        <v>1</v>
+      </c>
+      <c r="H24" s="4">
+        <v>-0.11</v>
+      </c>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4">
+        <v>623</v>
+      </c>
+      <c r="C25" s="3">
+        <v>50</v>
+      </c>
+      <c r="D25" s="5">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E25" s="4">
+        <v>100</v>
+      </c>
+      <c r="F25" s="6">
+        <v>4.05</v>
+      </c>
+      <c r="G25" s="11">
+        <v>1</v>
+      </c>
+      <c r="H25" s="7">
+        <v>-9.4500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4">
+        <v>623</v>
+      </c>
+      <c r="C26" s="3">
+        <v>50</v>
+      </c>
+      <c r="D26" s="5">
         <f>4</f>
         <v>4</v>
       </c>
-      <c r="E12" s="4">
-        <v>100</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="4">
-        <v>1</v>
-      </c>
-      <c r="H12" s="7">
+      <c r="E26" s="4">
+        <v>100</v>
+      </c>
+      <c r="F26" s="6">
+        <v>13.32</v>
+      </c>
+      <c r="G26" s="11">
+        <v>1</v>
+      </c>
+      <c r="H26" s="7">
         <v>-8.2900000000000001E-2</v>
       </c>
-      <c r="I12" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -977,37 +1327,37 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="I1" t="s">
         <v>1</v>
       </c>
       <c r="J1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="K1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="L1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="M1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>